<commit_message>
remove locale from workbook
the idea of storing a locale for the workbook was nice but caused more
problems than it solved, so locales were removed again.
</commit_message>
<xml_diff>
--- a/meja/src/test/resources/com/dua3/meja/text/FormatTest.xlsx
+++ b/meja/src/test/resources/com/dua3/meja/text/FormatTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="18060" windowHeight="11130"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="18060" windowHeight="11130" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NumberFormat" sheetId="2" r:id="rId1"/>
@@ -14,8 +14,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Wulff, Carsten (ext)</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alter Wert: 01.07.2017</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alter Wert: 01.07.2017</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>short user defined format</t>
   </si>
@@ -127,6 +163,18 @@
       <t xml:space="preserve"> conversion of custom formats is not yet implemented</t>
     </r>
   </si>
+  <si>
+    <t>01.10.1991</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>01.07.2017</t>
+  </si>
+  <si>
+    <t>(copied from Excel file)</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +187,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -173,6 +221,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +242,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -208,16 +268,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -229,6 +300,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -533,7 +620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -543,26 +630,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -573,7 +660,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -584,62 +671,62 @@
       <c r="B4">
         <v>1.2344999999999999</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>1.2354000000000001</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="4">
         <v>1.2356</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="4">
         <v>1.2343999999999999</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="4">
         <v>1.2345999999999999</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="5">
         <v>1.25</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D9" t="s">
@@ -647,13 +734,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="3">
         <v>1234567.8899999999</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -664,7 +751,7 @@
       <c r="B11">
         <v>1234567.8899999999</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -678,10 +765,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -690,26 +779,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="10" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -717,10 +806,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="9">
         <v>42795</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -728,10 +817,10 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="10">
         <v>42796</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -739,10 +828,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="11">
         <v>42797</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
@@ -753,14 +842,42 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="12">
         <v>42798</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="13">
+        <v>33512</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15">
+        <v>42917</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -769,5 +886,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test formatting for different locales
</commit_message>
<xml_diff>
--- a/meja/src/test/resources/com/dua3/meja/text/FormatTest.xlsx
+++ b/meja/src/test/resources/com/dua3/meja/text/FormatTest.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="18060" windowHeight="11130" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="60" windowWidth="18060" windowHeight="11130"/>
   </bookViews>
   <sheets>
-    <sheet name="NumberFormat" sheetId="2" r:id="rId1"/>
-    <sheet name="DateFormat" sheetId="1" r:id="rId2"/>
+    <sheet name="standard tests" sheetId="1" r:id="rId1"/>
+    <sheet name="regressions" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -20,7 +20,7 @@
     <author>Wulff, Carsten (ext)</author>
   </authors>
   <commentList>
-    <comment ref="B8" authorId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -33,7 +33,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
   <si>
     <t>short user defined format</t>
   </si>
@@ -131,49 +131,79 @@
     <t>1,3</t>
   </si>
   <si>
-    <t>Note that 1,25 has an exact representation as double</t>
-  </si>
-  <si>
     <t>remarks</t>
   </si>
   <si>
-    <t>#IGNORE#</t>
-  </si>
-  <si>
-    <t>Note that this workbook is using the german locale, so the formatting may look unusual.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>#IGNORE#</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> conversion of custom formats is not yet implemented</t>
-    </r>
-  </si>
-  <si>
     <t>01.10.1991</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>01.07.2017</t>
   </si>
   <si>
-    <t>(copied from Excel file)</t>
+    <t>Locale</t>
+  </si>
+  <si>
+    <t>date formats</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>ignored</t>
+  </si>
+  <si>
+    <t>number formats</t>
+  </si>
+  <si>
+    <t>conversion of custom formats is not yet implemented</t>
+  </si>
+  <si>
+    <t>1,25 - Note that 1,25 has an exact double representation</t>
+  </si>
+  <si>
+    <t>wrong display</t>
+  </si>
+  <si>
+    <t>de-DE</t>
+  </si>
+  <si>
+    <t>en-US</t>
+  </si>
+  <si>
+    <t>1234567.89</t>
+  </si>
+  <si>
+    <t>1,234,567.89</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>1.235</t>
+  </si>
+  <si>
+    <t>1.234</t>
+  </si>
+  <si>
+    <t>1.236</t>
+  </si>
+  <si>
+    <t>1.2345</t>
+  </si>
+  <si>
+    <t>Mar 1, 2017</t>
+  </si>
+  <si>
+    <t>Thursday, March 2, 2017</t>
+  </si>
+  <si>
+    <t>3/ March 2017</t>
+  </si>
+  <si>
+    <t>04/03/17</t>
+  </si>
+  <si>
+    <t>the order of fields is defined in format</t>
   </si>
 </sst>
 </file>
@@ -187,7 +217,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -203,19 +233,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="3" tint="0.39997558519241921"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="3" tint="0.39997558519241921"/>
       <name val="Arial"/>
@@ -234,37 +251,37 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -283,24 +300,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -311,12 +357,26 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -618,146 +678,501 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5">
+        <v>42795</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42796</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="7">
+        <v>42797</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="8">
+        <v>42798</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="5">
+        <v>42795</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42796</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="7">
+        <v>42797</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="8">
+        <v>42798</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="C12" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="F12" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
+      <c r="C13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13">
         <v>1.2344999999999999</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="15">
+        <v>1.2344999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.2354000000000001</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="15">
+        <v>1.2354000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.2356</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="15">
+        <v>1.2356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.2343999999999999</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="15">
+        <v>1.2343999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.2345999999999999</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="15">
+        <v>1.2345999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1234567.8899999999</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="15">
+        <v>1234567.8899999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>1234567.8899999999</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1234567.8899999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22">
+        <v>1.2344999999999999</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="F22" s="15">
+        <v>1.2344999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="4">
+      <c r="C23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3">
         <v>1.2354000000000001</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="F23" s="15">
+        <v>1.2354000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="4">
+      <c r="C24" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="3">
         <v>1.2356</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="F24" s="15">
+        <v>1.2356</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4">
+      <c r="C25" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="3">
         <v>1.2343999999999999</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="F25" s="15">
+        <v>1.2343999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4">
+      <c r="C26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="3">
         <v>1.2345999999999999</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="F26" s="15">
+        <v>1.2345999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5">
+      <c r="C27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="4">
         <v>1.25</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="F27" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="2">
         <v>1234567.8899999999</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="F28" s="15">
+        <v>1234567.8899999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="C29" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
         <v>1234567.8899999999</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F29" s="15">
+        <v>1234567.8899999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:C2"/>
+  <mergeCells count="2">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -766,126 +1181,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="9">
+        <v>33512</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="11">
+        <v>42917</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="9">
-        <v>42795</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10">
-        <v>42796</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11">
-        <v>42797</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="12">
-        <v>42798</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="13">
-        <v>33512</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="15">
-        <v>42917</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>